<commit_message>
GDD, analise de requisitos e casos de utilizacao atualizados
</commit_message>
<xml_diff>
--- a/doc/b01_02_requisitos_V3.xlsx
+++ b/doc/b01_02_requisitos_V3.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://iselpt-my.sharepoint.com/personal/diogo_lopes_isel_pt/Documents/Projects/45121_45125_Projecto/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luisc\Desktop\Faculdade\ProjetoFinal\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="34" documentId="13_ncr:40009_{929D2E82-99B8-4AB5-B604-D44E75EDAE35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2A93A37E-2705-4688-82C1-B0E7824FBCC7}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B768D2C-8316-4758-8361-332112F453A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="129">
   <si>
     <t>Visivel</t>
   </si>
@@ -113,22 +113,13 @@
     <t>R1.2</t>
   </si>
   <si>
-    <t>Transição nas diferentes cenas</t>
-  </si>
-  <si>
     <t>Invisível</t>
   </si>
   <si>
     <t>R1.3</t>
   </si>
   <si>
-    <t>Menu de escolher um planeta</t>
-  </si>
-  <si>
     <t>R1.4</t>
-  </si>
-  <si>
-    <t>Menu de escolher um nível</t>
   </si>
   <si>
     <t>R1.5</t>
@@ -163,9 +154,6 @@
     <t>R2.1</t>
   </si>
   <si>
-    <t>Área do jogo</t>
-  </si>
-  <si>
     <t>R2.2</t>
   </si>
   <si>
@@ -190,9 +178,6 @@
     <t>R2.5</t>
   </si>
   <si>
-    <t>Obtenção de recursos(reputação)</t>
-  </si>
-  <si>
     <t>R2.6</t>
   </si>
   <si>
@@ -202,66 +187,39 @@
     <t>R2.7</t>
   </si>
   <si>
-    <t>Construír mais naves, usando os recursos fornecidos</t>
-  </si>
-  <si>
     <t>R2.8</t>
   </si>
   <si>
     <t>R2.9</t>
   </si>
   <si>
-    <t>Atribuição de diferentes atributos(vida, poder de ataque) às naves</t>
-  </si>
-  <si>
     <t>R2.10</t>
   </si>
   <si>
-    <t>Verificação da condição de Vitória e Fim do Jogo</t>
-  </si>
-  <si>
     <t>R2.11</t>
   </si>
   <si>
-    <t>Aperfeiçoamento do mapa</t>
-  </si>
-  <si>
     <t>R3.1</t>
   </si>
   <si>
-    <t>O jogo deverá reproduzir músicas</t>
-  </si>
-  <si>
     <t>R3.2 </t>
   </si>
   <si>
-    <t>O jogo deverá mudar a música consoante o contexto de combate </t>
-  </si>
-  <si>
     <t>Adorno </t>
   </si>
   <si>
     <t>R3.3 </t>
   </si>
   <si>
-    <t>Os ataques do jogador devem reproduzir sons adequados, tanto ao infligir como ao receber danos </t>
-  </si>
-  <si>
     <t>Evidente </t>
   </si>
   <si>
     <t>R3.4 </t>
   </si>
   <si>
-    <t>Os ataques dos inimigos devem reproduzir sons adequados, tanto ao infligir como ao receber danos </t>
-  </si>
-  <si>
     <t>R3.5</t>
   </si>
   <si>
-    <t>Deve ser possível mudar o volume do som </t>
-  </si>
-  <si>
     <t>R4.1 </t>
   </si>
   <si>
@@ -283,48 +241,27 @@
     <t>R4.4 </t>
   </si>
   <si>
-    <t>O valor da reputação cresce consoante o tempo e os inimigos derrotados no jogo</t>
-  </si>
-  <si>
     <t>R4.5 </t>
   </si>
   <si>
     <t>Mostrar botões de construir mais naves no jogo</t>
   </si>
   <si>
-    <t>R4.6 </t>
-  </si>
-  <si>
-    <t>Selecionar botões para construir mais naves</t>
-  </si>
-  <si>
     <t>R5.1 </t>
   </si>
   <si>
-    <t>Um inimigo deverá ter um sistema de visão </t>
-  </si>
-  <si>
     <t>Invisível </t>
   </si>
   <si>
     <t>R5.2 </t>
   </si>
   <si>
-    <t>Um inimigo deve conseguir perseguir o jogador </t>
-  </si>
-  <si>
     <t>R5.3 </t>
   </si>
   <si>
-    <t>Um inimigo deve poder atacar o personagem </t>
-  </si>
-  <si>
     <t>R5.4</t>
   </si>
   <si>
-    <t>Um inimigo deve poder patrulhar uma rota predefinida </t>
-  </si>
-  <si>
     <t>R6.1 </t>
   </si>
   <si>
@@ -338,9 +275,6 @@
   </si>
   <si>
     <t>R6.3 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Portais que a cada 60 segundos faz spawn de uma nave aleatória (nave mãe excluída) </t>
   </si>
   <si>
     <t>R6.4 </t>
@@ -436,21 +370,12 @@
     <t>Consoante o número de recursos, o jogador pode construir mais naves</t>
   </si>
   <si>
-    <t>Uso exclusivo do rato</t>
-  </si>
-  <si>
     <t>Resposta rápida do jogo</t>
   </si>
   <si>
     <t>Plataforma</t>
   </si>
   <si>
-    <t>Windows NT</t>
-  </si>
-  <si>
-    <t>Android</t>
-  </si>
-  <si>
     <t>Desempenho</t>
   </si>
   <si>
@@ -461,9 +386,6 @@
   </si>
   <si>
     <t>Estética</t>
-  </si>
-  <si>
-    <t>Os menus devem ser adequados ao contexto do jogo</t>
   </si>
   <si>
     <t>Dificuldade do jogo</t>
@@ -512,6 +434,96 @@
   </si>
   <si>
     <t>Animações do jogador e das naves</t>
+  </si>
+  <si>
+    <t>Visualizar a área do jogo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Portais que a cada 60 segundos geram uma nave aleatória (nave mãe excluída) </t>
+  </si>
+  <si>
+    <t>Uso do rato e do teclado</t>
+  </si>
+  <si>
+    <t>Windows 10 e 11</t>
+  </si>
+  <si>
+    <t>Efetuar a transição nas diferentes cenas</t>
+  </si>
+  <si>
+    <t>Mostrar menu de escolher um planeta</t>
+  </si>
+  <si>
+    <t>Mostrar menu de escolher um nível</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Menus </t>
+  </si>
+  <si>
+    <t>Jogabilidade</t>
+  </si>
+  <si>
+    <t>Som</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interface </t>
+  </si>
+  <si>
+    <t>IA</t>
+  </si>
+  <si>
+    <t>Regras</t>
+  </si>
+  <si>
+    <t>Obter recursos(reputação)</t>
+  </si>
+  <si>
+    <t>Atribuir  diferentes atributos(vida, poder de ataque,velocidade) às naves</t>
+  </si>
+  <si>
+    <t>Verificar condição de Vitória e Fim do Jogo</t>
+  </si>
+  <si>
+    <t>Aperfeiçoar o mapa</t>
+  </si>
+  <si>
+    <t>Reproduzir músicas</t>
+  </si>
+  <si>
+    <t>Mudar a música consoante o contexto de combate </t>
+  </si>
+  <si>
+    <t>Mudar o volume do som </t>
+  </si>
+  <si>
+    <t>Reproduzir sons adequados, tanto ao infligir como ao receber danos (inimigo)</t>
+  </si>
+  <si>
+    <t>Rerproduzir sons adequados, tanto ao infligir como ao receber danos (jogador)</t>
+  </si>
+  <si>
+    <t>Incremar a reputação consoante o tempo e os inimigos derrotados no jogo</t>
+  </si>
+  <si>
+    <t>Ter um sistema de visão </t>
+  </si>
+  <si>
+    <t>Conseguir perseguir outras naves</t>
+  </si>
+  <si>
+    <t>Atacar outras naves</t>
+  </si>
+  <si>
+    <t>Patrulhar uma rota predefinida </t>
+  </si>
+  <si>
+    <t>O ambiente deve estar adequado ao tema do jogo</t>
+  </si>
+  <si>
+    <t>Os menus devem ser adequados ao tema do jogo</t>
+  </si>
+  <si>
+    <t>As naves deve estar adequado ao tema do jogo</t>
   </si>
 </sst>
 </file>
@@ -572,7 +584,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="55">
+  <borders count="69">
     <border>
       <left/>
       <right/>
@@ -1016,19 +1028,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color theme="1"/>
-      </right>
-      <top style="thin">
-        <color indexed="22"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="22"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -1162,19 +1161,6 @@
     </border>
     <border>
       <left style="medium">
-        <color theme="1"/>
-      </left>
-      <right style="medium">
-        <color theme="1"/>
-      </right>
-      <top style="thin">
-        <color indexed="22"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="medium">
@@ -1290,13 +1276,229 @@
       <bottom style="thin">
         <color indexed="22"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1"/>
+      </left>
+      <right style="medium">
+        <color theme="1"/>
+      </right>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="22"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="22"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="22"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="22"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="22"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="22"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="22"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1351,7 +1553,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1369,59 +1570,101 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="38" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="58" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="61" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="59" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="64" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="65" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="67" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="66" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2498,10 +2741,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2513,7 +2756,7 @@
     <col min="5" max="5" width="13.5546875" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1"/>
       <c r="C1"/>
       <c r="D1" s="11" t="s">
@@ -2521,7 +2764,7 @@
       </c>
       <c r="E1"/>
     </row>
-    <row r="2" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2"/>
       <c r="C2"/>
       <c r="D2" s="11" t="s">
@@ -2529,7 +2772,7 @@
       </c>
       <c r="E2"/>
     </row>
-    <row r="3" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3"/>
       <c r="C3"/>
       <c r="D3" s="11" t="s">
@@ -2537,530 +2780,586 @@
       </c>
       <c r="E3"/>
     </row>
-    <row r="4" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4"/>
       <c r="C4"/>
       <c r="D4" s="11"/>
       <c r="E4"/>
     </row>
-    <row r="5" spans="2:5" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:6" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5"/>
       <c r="C5"/>
       <c r="D5" s="11"/>
       <c r="E5"/>
     </row>
-    <row r="6" spans="2:5" s="1" customFormat="1" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="32" t="s">
+    <row r="6" spans="2:6" s="1" customFormat="1" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="31" t="s">
+      <c r="C6" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="30" t="s">
+      <c r="D6" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="29" t="s">
+      <c r="E6" s="81" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="2:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="48" t="s">
+      <c r="C7" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="33" t="s">
+      <c r="D7" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="25"/>
-    </row>
-    <row r="8" spans="2:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E7" s="82" t="s">
+        <v>106</v>
+      </c>
+      <c r="F7" s="80"/>
+    </row>
+    <row r="8" spans="2:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D8" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="50" t="s">
+      <c r="E8" s="83"/>
+      <c r="F8" s="80"/>
+    </row>
+    <row r="9" spans="2:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="36"/>
-    </row>
-    <row r="9" spans="2:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="5" t="s">
+      <c r="C9" s="46" t="s">
+        <v>104</v>
+      </c>
+      <c r="D9" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="83"/>
+      <c r="F9" s="80"/>
+    </row>
+    <row r="10" spans="2:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="48" t="s">
+      <c r="C10" s="58" t="s">
+        <v>105</v>
+      </c>
+      <c r="D10" s="55" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="83"/>
+      <c r="F10" s="80"/>
+    </row>
+    <row r="11" spans="2:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="37" t="s">
+      <c r="C11" s="57" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="36"/>
-    </row>
-    <row r="10" spans="2:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="60" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="62" t="s">
+      <c r="E11" s="83"/>
+      <c r="F11" s="80"/>
+    </row>
+    <row r="12" spans="2:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="58" t="s">
+      <c r="C12" s="50" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="59"/>
-    </row>
-    <row r="11" spans="2:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="49" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="61" t="s">
+      <c r="E12" s="83"/>
+      <c r="F12" s="80"/>
+    </row>
+    <row r="13" spans="2:6" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="57" t="s">
+      <c r="C13" s="52" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="86" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="7"/>
-    </row>
-    <row r="12" spans="2:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="50" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="53" t="s">
+      <c r="E13" s="85"/>
+      <c r="F13" s="80"/>
+    </row>
+    <row r="14" spans="2:6" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="41"/>
+      <c r="C14" s="42"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="42"/>
+    </row>
+    <row r="15" spans="2:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="57" t="s">
+      <c r="C15" s="34" t="s">
+        <v>99</v>
+      </c>
+      <c r="D15" s="37" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="2:5" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="52" t="s">
+      <c r="E15" s="88" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="55" t="s">
+      <c r="C16" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="56" t="s">
+      <c r="D16" s="33" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="14" spans="2:5" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="43"/>
-      <c r="C14" s="44"/>
-      <c r="D14" s="44"/>
-    </row>
-    <row r="15" spans="2:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" s="35" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" s="39" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D16" s="34" t="s">
-        <v>9</v>
-      </c>
+      <c r="E16" s="83"/>
     </row>
     <row r="17" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D17" s="34" t="s">
-        <v>29</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="D17" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="83"/>
     </row>
     <row r="18" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D18" s="49" t="s">
-        <v>12</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="D18" s="47" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="83"/>
     </row>
     <row r="19" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D19" s="34" t="s">
+        <v>112</v>
+      </c>
+      <c r="D19" s="33" t="s">
         <v>9</v>
       </c>
+      <c r="E19" s="83"/>
     </row>
     <row r="20" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D20" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" s="33" t="s">
         <v>9</v>
       </c>
+      <c r="E20" s="83"/>
     </row>
     <row r="21" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D21" s="34" t="s">
+        <v>97</v>
+      </c>
+      <c r="D21" s="33" t="s">
         <v>9</v>
       </c>
+      <c r="E21" s="83"/>
     </row>
     <row r="22" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="D22" s="34" t="s">
+        <v>98</v>
+      </c>
+      <c r="D22" s="33" t="s">
         <v>9</v>
       </c>
+      <c r="E22" s="83"/>
     </row>
     <row r="23" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D23" s="49" t="s">
-        <v>12</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="D23" s="47" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" s="83"/>
     </row>
     <row r="24" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D24" s="34" t="s">
+        <v>114</v>
+      </c>
+      <c r="D24" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="E24" s="59"/>
-    </row>
-    <row r="25" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E24" s="83"/>
+    </row>
+    <row r="25" spans="1:5" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="24"/>
-      <c r="B25" s="40" t="s">
-        <v>43</v>
-      </c>
-      <c r="C25" s="40" t="s">
-        <v>44</v>
-      </c>
-      <c r="D25" s="42" t="s">
+      <c r="B25" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="C25" s="38" t="s">
+        <v>115</v>
+      </c>
+      <c r="D25" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="E25" s="25"/>
-    </row>
-    <row r="26" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="45"/>
-      <c r="C26" s="46"/>
-      <c r="D26" s="46"/>
-      <c r="E26" s="36"/>
+      <c r="E25" s="83"/>
+    </row>
+    <row r="26" spans="1:5" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="43"/>
+      <c r="C26" s="44"/>
+      <c r="D26" s="44"/>
+      <c r="E26" s="89"/>
     </row>
     <row r="27" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D27" s="34" t="s">
+        <v>116</v>
+      </c>
+      <c r="D27" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="E27" s="36"/>
+      <c r="E27" s="88" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="28" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="26"/>
       <c r="B28" s="5" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D28" s="34" t="s">
-        <v>49</v>
-      </c>
-      <c r="E28" s="36"/>
+        <v>117</v>
+      </c>
+      <c r="D28" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="E28" s="83"/>
     </row>
     <row r="29" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="27"/>
       <c r="B29" s="5" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D29" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="E29" s="36"/>
+        <v>119</v>
+      </c>
+      <c r="D29" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="E29" s="83"/>
     </row>
     <row r="30" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="27"/>
       <c r="B30" s="5" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="D30" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="E30" s="36"/>
-    </row>
-    <row r="31" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="41" t="s">
-        <v>55</v>
-      </c>
-      <c r="C31" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="D31" s="42" t="s">
-        <v>52</v>
-      </c>
-      <c r="E31" s="36"/>
+        <v>120</v>
+      </c>
+      <c r="D30" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="E30" s="83"/>
+    </row>
+    <row r="31" spans="1:5" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="C31" s="38" t="s">
+        <v>118</v>
+      </c>
+      <c r="D31" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="E31" s="90"/>
     </row>
     <row r="32" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="63"/>
-      <c r="C32" s="63"/>
-      <c r="D32" s="63"/>
-      <c r="E32" s="36"/>
-    </row>
-    <row r="33" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="59"/>
+      <c r="C32" s="59"/>
+      <c r="D32" s="59"/>
+      <c r="E32" s="59"/>
+    </row>
+    <row r="33" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="27"/>
       <c r="B33" s="5" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D33" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="D33" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="E33" s="92" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D34" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="E34" s="83"/>
+    </row>
+    <row r="35" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C35" s="46" t="s">
+        <v>48</v>
+      </c>
+      <c r="D35" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="E35" s="83"/>
+    </row>
+    <row r="36" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C36" s="46" t="s">
+        <v>121</v>
+      </c>
+      <c r="D36" s="47" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36" s="83"/>
+    </row>
+    <row r="37" spans="1:6" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C37" s="46" t="s">
+        <v>51</v>
+      </c>
+      <c r="D37" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="E37" s="90"/>
+    </row>
+    <row r="38" spans="1:6" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="60"/>
+      <c r="C38" s="60"/>
+      <c r="D38" s="60"/>
+      <c r="E38" s="60"/>
+    </row>
+    <row r="39" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="E33" s="36"/>
-    </row>
-    <row r="34" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D34" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="E34" s="36"/>
-    </row>
-    <row r="35" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C35" s="48" t="s">
-        <v>62</v>
-      </c>
-      <c r="D35" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="E35" s="36"/>
-    </row>
-    <row r="36" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C36" s="48" t="s">
-        <v>64</v>
-      </c>
-      <c r="D36" s="49" t="s">
-        <v>12</v>
-      </c>
-      <c r="E36" s="36"/>
-    </row>
-    <row r="37" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C37" s="48" t="s">
-        <v>66</v>
-      </c>
-      <c r="D37" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="E37" s="36"/>
-    </row>
-    <row r="38" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="40" t="s">
-        <v>67</v>
-      </c>
-      <c r="C38" s="51" t="s">
-        <v>68</v>
-      </c>
-      <c r="D38" s="52" t="s">
-        <v>12</v>
-      </c>
-      <c r="E38" s="38"/>
-    </row>
-    <row r="39" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="64"/>
-      <c r="C39" s="64"/>
-      <c r="D39" s="64"/>
-      <c r="E39" s="28"/>
-    </row>
-    <row r="40" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C39" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="D39" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="E39" s="93" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="27"/>
       <c r="B40" s="5" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="D40" s="34" t="s">
-        <v>71</v>
-      </c>
-      <c r="E40" s="28"/>
-    </row>
-    <row r="41" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+      <c r="D40" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="E40" s="94"/>
+      <c r="F40" s="91"/>
+    </row>
+    <row r="41" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="27"/>
       <c r="B41" s="5" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="D41" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="E41" s="28"/>
-    </row>
-    <row r="42" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+      <c r="D41" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="E41" s="94"/>
+    </row>
+    <row r="42" spans="1:6" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="27"/>
-      <c r="B42" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="D42" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="E42" s="28"/>
-    </row>
-    <row r="43" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="62" t="s">
+        <v>56</v>
+      </c>
+      <c r="C42" s="61" t="s">
+        <v>125</v>
+      </c>
+      <c r="D42" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="E42" s="95"/>
+    </row>
+    <row r="43" spans="1:6" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="27"/>
-      <c r="B43" s="66" t="s">
-        <v>76</v>
-      </c>
-      <c r="C43" s="65" t="s">
-        <v>77</v>
-      </c>
-      <c r="D43" s="42" t="s">
-        <v>52</v>
-      </c>
-      <c r="E43" s="36"/>
-    </row>
-    <row r="44" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="60"/>
+      <c r="C43" s="60"/>
+      <c r="D43" s="87"/>
+      <c r="E43" s="87"/>
+    </row>
+    <row r="44" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="27"/>
-      <c r="B44" s="64"/>
-      <c r="C44" s="64"/>
-      <c r="D44" s="67"/>
-      <c r="E44" s="36"/>
-    </row>
-    <row r="45" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="46" t="s">
+        <v>57</v>
+      </c>
+      <c r="C44" s="46" t="s">
+        <v>58</v>
+      </c>
+      <c r="D44" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="E44" s="82" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="27"/>
-      <c r="B45" s="48" t="s">
-        <v>78</v>
-      </c>
-      <c r="C45" s="48" t="s">
-        <v>79</v>
-      </c>
-      <c r="D45" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="E45" s="36"/>
-    </row>
-    <row r="46" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="46" t="s">
+        <v>59</v>
+      </c>
+      <c r="C45" s="46" t="s">
+        <v>60</v>
+      </c>
+      <c r="D45" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="E45" s="83"/>
+    </row>
+    <row r="46" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="27"/>
-      <c r="B46" s="48" t="s">
-        <v>80</v>
-      </c>
-      <c r="C46" s="48" t="s">
-        <v>81</v>
-      </c>
-      <c r="D46" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="E46" s="36"/>
-    </row>
-    <row r="47" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="46" t="s">
+        <v>61</v>
+      </c>
+      <c r="C46" s="46" t="s">
+        <v>100</v>
+      </c>
+      <c r="D46" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="E46" s="83"/>
+    </row>
+    <row r="47" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="27"/>
-      <c r="B47" s="48" t="s">
-        <v>82</v>
-      </c>
-      <c r="C47" s="48" t="s">
-        <v>83</v>
-      </c>
-      <c r="D47" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="E47" s="36"/>
-    </row>
-    <row r="48" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="63" t="s">
+        <v>62</v>
+      </c>
+      <c r="C47" s="58" t="s">
+        <v>63</v>
+      </c>
+      <c r="D47" s="55" t="s">
+        <v>40</v>
+      </c>
+      <c r="E47" s="83"/>
+    </row>
+    <row r="48" spans="1:6" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="27"/>
-      <c r="B48" s="68" t="s">
-        <v>84</v>
-      </c>
-      <c r="C48" s="62" t="s">
-        <v>85</v>
-      </c>
-      <c r="D48" s="58" t="s">
-        <v>52</v>
-      </c>
-      <c r="E48" s="70"/>
+      <c r="B48" s="65" t="s">
+        <v>64</v>
+      </c>
+      <c r="C48" s="64" t="s">
+        <v>65</v>
+      </c>
+      <c r="D48" s="53" t="s">
+        <v>40</v>
+      </c>
+      <c r="E48" s="84"/>
     </row>
     <row r="49" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="27"/>
-      <c r="B49" s="72" t="s">
-        <v>86</v>
-      </c>
-      <c r="C49" s="71" t="s">
-        <v>87</v>
-      </c>
-      <c r="D49" s="56" t="s">
-        <v>52</v>
-      </c>
-      <c r="E49" s="69"/>
+      <c r="E49" s="96"/>
     </row>
     <row r="50" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E50" s="7"/>
+      <c r="E50" s="13"/>
     </row>
     <row r="51" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="5"/>
       <c r="C51" s="6"/>
       <c r="D51" s="6"/>
+      <c r="E51" s="14"/>
+    </row>
+    <row r="52" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E52" s="14"/>
+    </row>
+    <row r="53" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E53" s="14"/>
+    </row>
+    <row r="54" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E54" s="14"/>
+    </row>
+    <row r="55" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E55" s="14"/>
+    </row>
+    <row r="56" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E56" s="14"/>
+    </row>
+    <row r="57" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E57" s="14"/>
+    </row>
+    <row r="58" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E58" s="14"/>
+    </row>
+    <row r="59" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E59" s="14"/>
     </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="E7:E13"/>
+    <mergeCell ref="E15:E25"/>
+    <mergeCell ref="E27:E31"/>
+    <mergeCell ref="E33:E37"/>
+    <mergeCell ref="E39:E42"/>
+    <mergeCell ref="E44:E48"/>
+  </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <dataValidations count="2">
     <dataValidation errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="Requisitos" error="Esse valor não pertence à lista." promptTitle="Requisitos" prompt="Escolha um valor da lista." sqref="D1:D6" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
@@ -3079,10 +3378,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D48"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView topLeftCell="A22" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26:G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3097,14 +3396,14 @@
       <c r="B1"/>
       <c r="C1"/>
       <c r="D1" s="11" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2"/>
       <c r="C2"/>
       <c r="D2" s="11" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3123,254 +3422,263 @@
       <c r="D5" s="11"/>
     </row>
     <row r="6" spans="1:4" s="1" customFormat="1" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="73" t="s">
-        <v>90</v>
-      </c>
-      <c r="C6" s="76" t="s">
-        <v>91</v>
-      </c>
-      <c r="D6" s="29" t="s">
-        <v>92</v>
+      <c r="B6" s="66" t="s">
+        <v>68</v>
+      </c>
+      <c r="C6" s="69" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" s="28" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="37" t="s">
-        <v>93</v>
-      </c>
-      <c r="C7" s="77" t="s">
-        <v>94</v>
-      </c>
-      <c r="D7" s="74" t="s">
-        <v>89</v>
+      <c r="B7" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" s="70" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" s="67" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="37"/>
-      <c r="C8" s="78" t="s">
-        <v>95</v>
-      </c>
-      <c r="D8" s="41"/>
+      <c r="B8" s="36"/>
+      <c r="C8" s="71" t="s">
+        <v>73</v>
+      </c>
+      <c r="D8" s="39"/>
     </row>
     <row r="9" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="37"/>
-      <c r="C9" s="79" t="s">
-        <v>94</v>
+      <c r="B9" s="36"/>
+      <c r="C9" s="72" t="s">
+        <v>72</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="42"/>
-      <c r="C10" s="78" t="s">
-        <v>96</v>
-      </c>
-      <c r="D10" s="75"/>
+      <c r="B10" s="40"/>
+      <c r="C10" s="71" t="s">
+        <v>74</v>
+      </c>
+      <c r="D10" s="68"/>
     </row>
     <row r="11" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="27"/>
-      <c r="B11" s="82" t="s">
-        <v>97</v>
-      </c>
-      <c r="C11" s="80" t="s">
-        <v>94</v>
+      <c r="B11" s="75" t="s">
+        <v>75</v>
+      </c>
+      <c r="C11" s="73" t="s">
+        <v>72</v>
       </c>
       <c r="D11" s="25" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="40"/>
+      <c r="C12" s="74" t="s">
+        <v>76</v>
+      </c>
+      <c r="D12" s="68"/>
+    </row>
+    <row r="13" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="C13" s="76" t="s">
+        <v>72</v>
+      </c>
+      <c r="D13" s="25" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="36"/>
+      <c r="C14" s="45" t="s">
+        <v>78</v>
+      </c>
+      <c r="D14" s="68"/>
+    </row>
+    <row r="15" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="36"/>
+      <c r="C15" s="72" t="s">
+        <v>72</v>
+      </c>
+      <c r="D15" s="25" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="36"/>
+      <c r="C16" s="45" t="s">
+        <v>79</v>
+      </c>
+      <c r="D16" s="39"/>
+    </row>
+    <row r="17" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="36"/>
+      <c r="C17" s="72" t="s">
+        <v>72</v>
+      </c>
+      <c r="D17" s="25" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="36"/>
+      <c r="C18" s="45" t="s">
+        <v>80</v>
+      </c>
+      <c r="D18" s="39"/>
+    </row>
+    <row r="19" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="36"/>
+      <c r="C19" s="77" t="s">
+        <v>72</v>
+      </c>
+      <c r="D19" s="25" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="55"/>
+      <c r="C20" s="71" t="s">
+        <v>101</v>
+      </c>
+      <c r="D20" s="68"/>
+    </row>
+    <row r="21" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="C21" s="70" t="s">
+        <v>72</v>
+      </c>
+      <c r="D21" s="35" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="36"/>
+      <c r="C22" s="45" t="s">
+        <v>102</v>
+      </c>
+      <c r="D22" s="68"/>
+    </row>
+    <row r="23" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="51" t="s">
+        <v>83</v>
+      </c>
+      <c r="C23" s="73" t="s">
+        <v>84</v>
+      </c>
+      <c r="D23" s="25" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="40"/>
+      <c r="C24" s="74" t="s">
+        <v>85</v>
+      </c>
+      <c r="D24" s="68"/>
+    </row>
+    <row r="25" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C25" s="77" t="s">
+        <v>72</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C26" s="71" t="s">
+        <v>81</v>
+      </c>
+      <c r="D26" s="68"/>
+    </row>
+    <row r="27" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="51" t="s">
+        <v>86</v>
+      </c>
+      <c r="C27" s="78" t="s">
+        <v>72</v>
+      </c>
+      <c r="D27" s="25" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="40"/>
+      <c r="C28" s="52" t="s">
+        <v>127</v>
+      </c>
+      <c r="D28" s="68"/>
+    </row>
+    <row r="29" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="97"/>
+      <c r="C29" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="D29" s="25" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="98"/>
+      <c r="C30" s="101" t="s">
+        <v>126</v>
+      </c>
+      <c r="D30" s="100"/>
+    </row>
+    <row r="31" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="99"/>
+      <c r="C31" s="103" t="s">
+        <v>72</v>
+      </c>
+      <c r="D31" s="25" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="101"/>
+      <c r="C32" s="101" t="s">
+        <v>128</v>
+      </c>
+      <c r="D32" s="102"/>
+    </row>
+    <row r="33" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="51" t="s">
+        <v>87</v>
+      </c>
+      <c r="C33" s="79" t="s">
+        <v>72</v>
+      </c>
+      <c r="D33" s="25" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="40"/>
+      <c r="C34" s="71" t="s">
+        <v>88</v>
+      </c>
+      <c r="D34" s="68"/>
+    </row>
+    <row r="46" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="8" t="s">
         <v>89</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="42"/>
-      <c r="C12" s="81" t="s">
-        <v>98</v>
-      </c>
-      <c r="D12" s="75"/>
-    </row>
-    <row r="13" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="33" t="s">
-        <v>99</v>
-      </c>
-      <c r="C13" s="83" t="s">
-        <v>94</v>
-      </c>
-      <c r="D13" s="25" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="37"/>
-      <c r="C14" s="47" t="s">
-        <v>100</v>
-      </c>
-      <c r="D14" s="75"/>
-    </row>
-    <row r="15" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="37"/>
-      <c r="C15" s="79" t="s">
-        <v>94</v>
-      </c>
-      <c r="D15" s="25" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="37"/>
-      <c r="C16" s="47" t="s">
-        <v>101</v>
-      </c>
-      <c r="D16" s="41"/>
-    </row>
-    <row r="17" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="37"/>
-      <c r="C17" s="79" t="s">
-        <v>94</v>
-      </c>
-      <c r="D17" s="25" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="37"/>
-      <c r="C18" s="47" t="s">
-        <v>102</v>
-      </c>
-      <c r="D18" s="41"/>
-    </row>
-    <row r="19" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="37"/>
-      <c r="C19" s="84" t="s">
-        <v>94</v>
-      </c>
-      <c r="D19" s="25" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="58"/>
-      <c r="C20" s="78" t="s">
-        <v>103</v>
-      </c>
-      <c r="D20" s="75"/>
-    </row>
-    <row r="21" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="5"/>
-      <c r="C21" s="84" t="s">
-        <v>94</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="42"/>
-      <c r="C22" s="78" t="s">
-        <v>104</v>
-      </c>
-      <c r="D22" s="75"/>
-    </row>
-    <row r="23" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="33" t="s">
-        <v>105</v>
-      </c>
-      <c r="C23" s="77" t="s">
-        <v>94</v>
-      </c>
-      <c r="D23" s="36" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="37"/>
-      <c r="C24" s="47" t="s">
-        <v>106</v>
-      </c>
-      <c r="D24" s="75"/>
-    </row>
-    <row r="25" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="37"/>
-      <c r="C25" s="79" t="s">
-        <v>94</v>
-      </c>
-      <c r="D25" s="25" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="42"/>
-      <c r="C26" s="47" t="s">
-        <v>107</v>
-      </c>
-      <c r="D26" s="75"/>
-    </row>
-    <row r="27" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="54" t="s">
-        <v>108</v>
-      </c>
-      <c r="C27" s="80" t="s">
-        <v>109</v>
-      </c>
-      <c r="D27" s="25" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="28" spans="2:4" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="42"/>
-      <c r="C28" s="81" t="s">
-        <v>110</v>
-      </c>
-      <c r="D28" s="75"/>
-    </row>
-    <row r="29" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="54" t="s">
-        <v>111</v>
-      </c>
-      <c r="C29" s="85" t="s">
-        <v>94</v>
-      </c>
-      <c r="D29" s="25" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="30" spans="2:4" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="42"/>
-      <c r="C30" s="81" t="s">
-        <v>112</v>
-      </c>
-      <c r="D30" s="75"/>
-    </row>
-    <row r="31" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="54" t="s">
-        <v>113</v>
-      </c>
-      <c r="C31" s="86" t="s">
-        <v>94</v>
-      </c>
-      <c r="D31" s="25" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="32" spans="2:4" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="42"/>
-      <c r="C32" s="78" t="s">
-        <v>114</v>
-      </c>
-      <c r="D32" s="75"/>
-    </row>
-    <row r="33" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="5"/>
-      <c r="C33" s="13"/>
-      <c r="D33" s="7"/>
-    </row>
-    <row r="48" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="8" t="s">
-        <v>115</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <dataValidations count="2">
     <dataValidation errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="Requisitos" error="O valor não pertence à lista." sqref="D1:D6" xr:uid="{00000000-0002-0000-0100-000000000000}"/>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="Requisitos" error="O valor não pertence à lista." sqref="D23:D27 D44:D65536 D29:D34 D13:D21" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="Requisitos" error="O valor não pertence à lista." sqref="D42:D65534 D25 D13:D23 D33:D34 D27:D29 D31:D32" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>$D$1:$D$5</formula1>
     </dataValidation>
   </dataValidations>
@@ -3387,8 +3695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:G34"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView topLeftCell="A4" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D13" sqref="D11:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3453,121 +3761,121 @@
         <v>3</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>5</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
-        <v>117</v>
+        <v>91</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>9</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>99</v>
+        <v>77</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>94</v>
+        <v>72</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F8" s="14" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="2:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
-        <v>120</v>
+        <v>94</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>9</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>99</v>
+        <v>77</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>94</v>
+        <v>72</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F11" s="14" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="2:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="8" t="s">
-        <v>121</v>
+        <v>95</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>9</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>99</v>
+        <v>77</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>94</v>
+        <v>72</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="2:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F14" s="14" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16" spans="2:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="8" t="s">
-        <v>122</v>
+        <v>96</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>123</v>
+        <v>97</v>
       </c>
       <c r="D16" s="9" t="s">
         <v>9</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>99</v>
+        <v>77</v>
       </c>
       <c r="F16" s="14" t="s">
-        <v>94</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="6:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F17" s="14" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
     </row>
     <row r="34" spans="2:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="8" t="s">
-        <v>115</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>